<commit_message>
Started to add the react components
</commit_message>
<xml_diff>
--- a/DB_Seeds.xlsx
+++ b/DB_Seeds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vern2\sei-21\projects\ga-sei-project-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vern2\sei-21\projects\ga-sei-project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79E65A-3F98-48CA-B560-CB6323BB3CE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3C27A7-19B1-4AB8-853E-2C7E1B1BFECE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{56699EEE-A768-4D4B-B9A9-D6C6635385E0}"/>
+    <workbookView xWindow="192" yWindow="72" windowWidth="12396" windowHeight="12168" activeTab="1" xr2:uid="{56699EEE-A768-4D4B-B9A9-D6C6635385E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="91">
   <si>
     <t>First Name</t>
   </si>
@@ -56,16 +56,340 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>Haute Cabriere</t>
+  </si>
+  <si>
+    <t>Chardonnay Pinot Noir</t>
+  </si>
+  <si>
+    <t>Pinot Noir Rose</t>
+  </si>
+  <si>
+    <t>Pinot Noir Unwooded</t>
+  </si>
+  <si>
+    <t>Pinot Noir Reserve</t>
+  </si>
+  <si>
+    <t>Pierre Jourdan Brut</t>
+  </si>
+  <si>
+    <t>Pierre Jourdan Belle Rose</t>
+  </si>
+  <si>
+    <t>Pierre Jourdan Blanc De Blancs</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Varietal</t>
+  </si>
+  <si>
+    <t>First created in 1994 from the classic blend traditionally reserved for sparkling wines, our Chardonnay Pinot Noir was the first South African still wine produced in this style.</t>
+  </si>
+  <si>
+    <t>Chardonnay and Pinot Noir</t>
+  </si>
+  <si>
+    <t>An elegant dry rosé with aromas of strawberries and rose petals. Pairs well with salmon, oysters and sushi.</t>
+  </si>
+  <si>
+    <t>Pinot Noir</t>
+  </si>
+  <si>
+    <t>IMG URL</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2019/04/Pinot_Noir_Rose_2019_V1.jpg</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2016/05/Haute-Cabriere-Chardonnay-Pinot-Noir-2018-product.jpg</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2016/05/Haute-Cabriere-Pinot-Noir-Unwooded-2018-product.jpg</t>
+  </si>
+  <si>
+    <t>This Pinot Noir is a testament to Franschhoek’s suitability for growing this varietal. Can be matured for 5-8 years</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2016/05/HC-Pinot-Noir-Reserve-2015-new-cap-product.jpg</t>
+  </si>
+  <si>
+    <t>This unwooded style of Pinot Noir is light and elegant. Pairs well with duck, tuna and cured meats. Serve chilled.</t>
+  </si>
+  <si>
+    <t>Pierre Jourdan Brut is an elegant Méthode Cap Classique created from a blend of the classic varietals of Chardonnay and Pinot Noir.</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2016/05/Pierre-Jourdan-MCC-Brut-750ml.jpg</t>
+  </si>
+  <si>
+    <t>The Belle Rose is a fruity Méthode Cap Classique which owes its salmon pink colour to the Pinot Noir varietal.
+The palate reveals a lively presentation of rich strawberry and cherry flavours derived from Pinot Noir – with an elegant dry finish.</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2016/05/Pierre-Jourdan-MCC-Belle-Rose.jpg</t>
+  </si>
+  <si>
+    <t>A rich, full bodied Méthode Cap Classique, matured on the lees for up to seven years. This award-winning wine pairs well with creamy seafood dishes like mussels and salmon.</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2017/03/Pierre-Jourdan-Blanc-De-Blancs-MCC_Web.jpg</t>
+  </si>
+  <si>
+    <t>Pierre Jourdan Tranquille</t>
+  </si>
+  <si>
+    <t>Tranquille is a classic blend of Pinot Noir and Chardonnay. Pairs well with lighter dishes like salad and sushi.</t>
+  </si>
+  <si>
+    <t>Pinot Noir and Chardonnay</t>
+  </si>
+  <si>
+    <t>https://www.cabriere.co.za/wp-content/uploads/2017/03/Tranquille_2019.jpg</t>
+  </si>
+  <si>
+    <t>The Goose Wines</t>
+  </si>
+  <si>
+    <t>The Goose Sauvignon Blanc</t>
+  </si>
+  <si>
+    <t>The Goose Chardonnay</t>
+  </si>
+  <si>
+    <t>The Goose Shiraz</t>
+  </si>
+  <si>
+    <t>The Goose Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>The Goose Pinot Noir</t>
+  </si>
+  <si>
+    <t>The Goose Expression</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Sauvignon Blanc</t>
+  </si>
+  <si>
+    <t>Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>https://www.thegoosewines.com/wp-content/uploads/2018/08/The-Goose-Wines-Sauvignon-Blanc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+2016
+Chardonnay
+WINE STYLE
+An unwooded wine, with good natural acidity and superb structure which is easy drinking and refreshing.
+TASTING NOTES
+Fruit driven with peach and pineapple, and hints of melon and lemon blossom on the nose.  Experience an abundance of these vibrant fresh fruits on the palate, which is well balanced with rich butterscotch creaminess and a cool, crisp finish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINE STYLE
+Packaged in a traditional Riesling shaped bottle and quite appropriate
+really, as the acidity in our Sauvignon Blanc grapes are all natural,
+which culminates in a beautifully balanced and broad mouth feel so
+reminiscent of the great wines of Sancerre, Alsace and Mosel.
+TASTING NOTES
+The Goose Sauvignon Blanc is an exciting and unique tasting
+experience with tropical fruit flavours of guava on the nose.
+The wine lingers beautifully on the palate, with a complexity
+that showcases a typical cool-climate mineraliy with balanced
+acidity.
+Download full tasting notes
+FOOD PAIRING
+The Goose Sauvignon Blanc will partner well with most salads
+and fish dishes. A real treat with freshly caught tuna and sushi.
+</t>
+  </si>
+  <si>
+    <t>Shiraz</t>
+  </si>
+  <si>
+    <t>https://www.thegoosewines.com/wp-content/uploads/2018/08/The-Goose-Wines-Chardonnay.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINE STYLE
+The tannins are soft and ripe and the wine has a long, clean
+aftertaste with enough tannic grip to promise a good few
+years maturation potential.
+TASTING NOTES
+The Goose Shiraz has a ruby red colour, scented bouquet with
+abundant smoke and spice, delivering exceptional richness and
+a powerful full-bodied finish.
+Download full tasting notes
+FOOD PAIRING
+The Goose Shiraz will partner well with grilled meat, cheese, or
+even that delectable dark chocolate dessert.
+</t>
+  </si>
+  <si>
+    <t>https://www.thegoosewines.com/wp-content/uploads/2018/08/The-Goose-Wines-Shiraz.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINE STYLE
+The Goose Cabernet Sauvignon is a well-balanced wine with
+ripe tannins and a long, layered finish.
+TASTING NOTES
+The Goose Cabernet Sauvignon has a brilliant purple colour
+with a sweet nose of blackberries and hints of cherry.
+Download full tasting notes
+FOOD PAIRING
+Enjoy The Goose Cabernet Sauvignon with roast meats, pasta
+dishes or hearty stews.
+</t>
+  </si>
+  <si>
+    <t>https://www.thegoosewines.com/wp-content/uploads/2018/08/The-Goose-Wines-Cabernet-Sauvignon.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINE STYLE
+The Goose Pinot Noir is produced from rugged mountain vineyard
+in a cool climate, expressing the true characters of this famed and
+loved grape variety.
+TASTING NOTES
+The Goose Pinot Noir has bright red fruit notes and a touch of spice
+are underscored by an earthy forest floor nuance.
+FOOD PAIRING
+The Goose Pinot Noir will partner well with mushrooms, veal, pork,
+turkey or beef fillet
+</t>
+  </si>
+  <si>
+    <t>https://www.thegoosewines.com/wp-content/uploads/2018/08/The-Goose-Wines-Pinot-Noir.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINE STYLE
+Chosen from the best performing rows of cabernet sauvignon and shiraz, matured in French Oak for 12 – 18 months.  The fruit is characterised by intense forwardness and unique tannin structure.  The cool climate terrior means a long, even ripening period, resulting in grapes of intense fruit, balance, structure and elegance.
+TASTING NOTES
+An amalgam of berries, spice and wood integration and trademark herbaceous character and white pepper support.  A very soft wine on the palate, yet full bodies with huge compexity.  Designed to mature 10 years after vintage.
+FOOD PAIRING
+The Expression will partner with any heavy, rich meat dish to perfection.  Think Oxtail, stews, beef, steak or even game and venison.
+</t>
+  </si>
+  <si>
+    <t>https://www.thegoosewines.com/wp-content/uploads/2018/08/The-Goose-Wines-Expression.png</t>
+  </si>
+  <si>
+    <t>Zevenwacht Wine Estate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Zevenwacht Z 360° Sauvignon Blanc 2018 </t>
+  </si>
+  <si>
+    <t>The nose shows concentrated aromas of nettles, crushed figand passion fruit, with hints of grapefruit that continues on tothe palate. The generous mouth feel is supported with a fine natural lime acidity that gives the wine length and focus. Previous vintages confirm that this wine ages beautifully and develops more complexity over time as flavours subtly change.</t>
+  </si>
+  <si>
+    <t>http://images.wine.co.za/GetWineImage.ashx?IMAGEID=264382&amp;ImageSize=small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Zevenwacht Z Gewürztraminer 2016 </t>
+  </si>
+  <si>
+    <t>Aromatic and intense the wine has delightful flavours of rose petals, litchi and Turkish delight. The wine has a full palate that is carried by a fresh acidity and lingering creamy finish.</t>
+  </si>
+  <si>
+    <t>http://images.wine.co.za/GetWineImage.ashx?IMAGEID=263553&amp;ImageSize=small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Zevenwacht Z Collection Reserve 2014 </t>
+  </si>
+  <si>
+    <t>Rich and generous, this wine boasts a deep dark hue and whiffs of ripe black currant infused with roasted coffee beans, tobacco leaves, cedar wood and cigar box. On the palate expect concentrated black plum and a decadent dark chocolate finish.</t>
+  </si>
+  <si>
+    <t>http://images.wine.co.za/GetWineImage.ashx?IMAGEID=262570&amp;ImageSize=small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Zevenwacht 7even Sauvignon Blanc 2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zevenwacht 7even Rood 2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zevenwacht 7even Syrah 2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zevenwacht 7even Bouquet Blanc 2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Zevenwacht 7even Rosé 2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zevenwacht 7even Pinotage 2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zevenwacht The Tin Mine White 2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zevenwacht The Tin Mine Red 2015 </t>
+  </si>
+  <si>
+    <t>Purple red in colour, with the nose that exudes aromas of violets, dried spices and concentrated black prunes with a slow release of red cranberry and dark chocolate. The palate impresses with density on entry matched with persistent yet supple tannins - a multi layered wine. This texture is perfectly offset by balanced acidity that allows for a remarkable length of finish.</t>
+  </si>
+  <si>
+    <t>Ripe and exotic, a distinctive, spicy, perfumed wine that is rich and subtly oaked. Complex aromas of dried yellow fruits and spice with a refreshing lime and citrus finish.</t>
+  </si>
+  <si>
+    <t>A wine with a delicate, beautiful salmon pink colour. Rose petals on the nose with fresh ripe strawberries on the palate - a long lingering fresh taste. A delicious lifestyle wine, elegant and soft</t>
+  </si>
+  <si>
+    <t>The nose has ripe plum and dark cherry fruit, complimented with chocolate and toasted coffee aromas. The palate is medium bodied and juicy with a smooth finish.</t>
+  </si>
+  <si>
+    <t>A perfumed nose with lots of fruit, floral and spicy aromas. Flavours of litchi, lime and yellow fruit. A complex aromatic wine, with well-balanced sugar and acidity, this wine provides a long crisp finish with layers of fruit and floral tones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A luscious lifestyle wine with hints of red raspberry fruit and white pepper spice, giving a first impression of red berries and chocolate with slight cedar wood undertones. Soft pliable tannins lend subtle support to the structure, yet are unobtrusive on the succulent palate. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An elegant, refreshing but fruit driven wine. A perfect combination of greener sweeter fruits with a beautiful density on the palate and a zesty lime citrus finish. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,18 +427,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,16 +770,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C62C6E-F83C-41AB-9AB5-9F4493C82485}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="15.7109375" customWidth="1"/>
+    <col min="1" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -491,12 +832,395 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E83AB71-05BD-4B69-A93B-28B622D59005}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="113.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{3AF11011-F8D7-403B-9321-11C4E119778F}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{DE04F767-B570-4EFE-BBD6-5F2706F933F0}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{6F01772F-E31C-4791-9224-523222FEB33A}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{358228A3-1A30-47DB-B2C5-617BF0DD1379}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{FDF571F4-E1C4-489C-B267-20D41635D8D8}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{5EDA32EB-1A77-4082-8D5A-813D8B548605}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{CEB495B8-2B2E-4240-8EEC-495418A0B1E9}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{354D0C9A-BED0-443F-969C-668A9A0195F0}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{28B8A3F3-DA0C-4DE0-992B-D9DD4E176AAB}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{4C142F1F-0FDF-43D6-BD11-194DED258DA5}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{676F4E8F-58AD-491E-B39E-6A1FE145F3DA}"/>
+    <hyperlink ref="E14" r:id="rId12" xr:uid="{A1CA1203-8A39-4C1D-9A5E-02EE5C4D2890}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{30A7866A-783C-4FE6-AE32-F865BF1F5F52}"/>
+    <hyperlink ref="E16" r:id="rId14" xr:uid="{9CD3719B-FBDB-4593-B138-F9A4855E22D4}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{05C8D4F2-AF0B-46B8-9878-B2B209BE0BAD}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{4DD06000-ED33-409E-9C2D-4D675AD0FFE1}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{0FBB1F9E-4E15-43CD-834D-CD9F7A91087D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>